<commit_message>
feat: turn Group required
</commit_message>
<xml_diff>
--- a/tests/data/output.xlsx
+++ b/tests/data/output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -46,10 +46,16 @@
     <t xml:space="preserve">After</t>
   </si>
   <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">iShares Core S&amp;P Total US Stock Market</t>
   </si>
   <si>
     <t xml:space="preserve">BITO39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
   </si>
   <si>
     <t xml:space="preserve">iShares Core MSCI EAFE</t>
@@ -145,13 +151,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -171,15 +181,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -204,56 +214,62 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="2" t="n">
         <v>1.11</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>0.5</v>
+      <c r="G2" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="2" t="n">
         <v>2.22</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="G3" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="2" t="n">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>